<commit_message>
"Turret & projectile v2"
</commit_message>
<xml_diff>
--- a/android/assets/spec.xlsx
+++ b/android/assets/spec.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>(Fast Firing)</t>
   </si>
@@ -232,6 +232,30 @@
   </si>
   <si>
     <t>gold is lost when bird passes through</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>XF</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>7+Diamond</t>
   </si>
 </sst>
 </file>
@@ -282,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -294,6 +318,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -834,19 +861,19 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" t="s">
         <v>59</v>
       </c>
       <c r="G10" t="s">
@@ -854,59 +881,163 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="A11" t="s">
         <v>54</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="1">
         <v>3</v>
       </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="C12">
+      <c r="B15" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13">
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>59</v>
       </c>
-      <c r="C16">
+      <c r="B17" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>60</v>
       </c>
-      <c r="C17">
+      <c r="B18" s="1">
         <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>